<commit_message>
update names of interventions
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Sept12/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Sept12/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6740" yWindow="-21140" windowWidth="18780" windowHeight="20560" tabRatio="500" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="-6660" yWindow="-21140" windowWidth="18780" windowHeight="20560" tabRatio="500" firstSheet="21" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -429,9 +429,6 @@
     <t>Intervention</t>
   </si>
   <si>
-    <t>Zinc supplementation</t>
-  </si>
-  <si>
     <t>Complements group</t>
   </si>
   <si>
@@ -447,9 +444,6 @@
     <t>Complementary feeding (food insecure with neither promotion nor supplementation)</t>
   </si>
   <si>
-    <t>Breastfeeding promotion (dual delivery)</t>
-  </si>
-  <si>
     <t>baseline coverage</t>
   </si>
   <si>
@@ -462,15 +456,6 @@
     <t>Vitamin A supplementation</t>
   </si>
   <si>
-    <t>Complementary feeding (education)</t>
-  </si>
-  <si>
-    <t>Complementary feeding (supplementation)</t>
-  </si>
-  <si>
-    <t>Balanced energy supplementation</t>
-  </si>
-  <si>
     <t>Multiple micronutrient supplementation</t>
   </si>
   <si>
@@ -496,6 +481,21 @@
   </si>
   <si>
     <t>fraction food insecure (not poor)</t>
+  </si>
+  <si>
+    <t>Prophylactic zinc supplementation</t>
+  </si>
+  <si>
+    <t>Breastfeeding promotion</t>
+  </si>
+  <si>
+    <t>Complementary feeding education</t>
+  </si>
+  <si>
+    <t>Public provision of complementary foods</t>
+  </si>
+  <si>
+    <t>Balanced energy-protein supplementation</t>
   </si>
 </sst>
 </file>
@@ -1171,6 +1171,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1541,7 +1592,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B5" s="13">
         <v>0.56799999999999995</v>
@@ -1549,7 +1600,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B6" s="26">
         <v>0.4</v>
@@ -1557,7 +1608,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B7" s="26">
         <v>0.20599999999999999</v>
@@ -2744,12 +2795,12 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="43.5" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2774,7 +2825,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
@@ -2835,7 +2886,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -2855,7 +2906,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
@@ -2875,7 +2926,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
@@ -2895,7 +2946,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -2915,7 +2966,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -2942,7 +2993,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2972,7 +3025,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="B2" s="18">
         <v>5.16</v>
@@ -3216,7 +3269,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3231,18 +3286,18 @@
         <v>56</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B2" s="20">
         <v>0</v>
@@ -3259,7 +3314,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="6">
         <v>0.621</v>
@@ -3276,7 +3331,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B4" s="6">
         <v>0.247</v>
@@ -3293,7 +3348,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B5" s="6">
         <v>0</v>
@@ -3310,7 +3365,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="B6" s="6">
         <v>0.61</v>
@@ -3327,7 +3382,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B7" s="6">
         <v>0</v>
@@ -3344,7 +3399,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -3466,7 +3521,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3499,14 +3554,14 @@
         <v>15</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -3529,7 +3584,7 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3552,7 +3607,7 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3575,7 +3630,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -3600,7 +3655,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
@@ -3623,7 +3678,7 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -3647,7 +3702,7 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
@@ -3777,12 +3832,12 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F5"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+    <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3790,7 +3845,7 @@
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
         <v>23</v>
@@ -3807,10 +3862,10 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C2" s="23">
         <v>0.21</v>
@@ -3827,7 +3882,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C3" s="23">
         <f>demographics!$B$5 * 'Interventions target population'!$G$7</f>
@@ -3846,10 +3901,10 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C4" s="23">
         <v>0.1</v>
@@ -3866,7 +3921,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C5" s="23">
         <v>1</v>
@@ -3891,17 +3946,17 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G5"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>10</v>
@@ -3924,7 +3979,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
@@ -3968,7 +4023,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>34</v>
@@ -4040,17 +4095,17 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G5"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>10</v>
@@ -4073,7 +4128,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
@@ -4117,7 +4172,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>34</v>
@@ -4188,18 +4243,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>10</v>
@@ -4222,7 +4277,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
@@ -4266,7 +4321,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>34</v>
@@ -4375,7 +4430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change several spreadsheet tab names, and one column title
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Sept12/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Sept12/InputForCode_Bangladesh.xlsx
@@ -9,27 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-6660" yWindow="-21140" windowWidth="18780" windowHeight="20560" tabRatio="500" firstSheet="21" activeTab="24"/>
+    <workbookView xWindow="-6660" yWindow="-21140" windowWidth="18800" windowHeight="20560" tabRatio="500" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
     <sheet name="projected births" sheetId="2" r:id="rId2"/>
-    <sheet name="total mortality" sheetId="3" r:id="rId3"/>
-    <sheet name="mortality" sheetId="4" r:id="rId4"/>
+    <sheet name="mortality rates" sheetId="3" r:id="rId3"/>
+    <sheet name="causes of death" sheetId="4" r:id="rId4"/>
     <sheet name="distributions" sheetId="5" r:id="rId5"/>
     <sheet name="birth outcome distribution" sheetId="6" r:id="rId6"/>
     <sheet name="Incidence of conditions" sheetId="7" r:id="rId7"/>
-    <sheet name="RRStunting" sheetId="8" r:id="rId8"/>
-    <sheet name="RRWasting" sheetId="9" r:id="rId9"/>
-    <sheet name="RRBreastfeeding" sheetId="10" r:id="rId10"/>
-    <sheet name="RR Death by Birth Outcome" sheetId="11" r:id="rId11"/>
+    <sheet name="RR death by stunting" sheetId="8" r:id="rId8"/>
+    <sheet name="RR death by wasting" sheetId="9" r:id="rId9"/>
+    <sheet name="RR death by breastfeeding" sheetId="10" r:id="rId10"/>
+    <sheet name="RR death by birth outcome" sheetId="11" r:id="rId11"/>
     <sheet name="OR stunting progression" sheetId="12" r:id="rId12"/>
     <sheet name="RR diarrhoea" sheetId="13" r:id="rId13"/>
     <sheet name="OR stunting by condition" sheetId="14" r:id="rId14"/>
     <sheet name="OR stunting by birth outcome" sheetId="15" r:id="rId15"/>
     <sheet name="OR stunting by intervention" sheetId="16" r:id="rId16"/>
-    <sheet name="OR stunting for complements" sheetId="17" r:id="rId17"/>
-    <sheet name="OR appropriateBF by interv" sheetId="18" r:id="rId18"/>
+    <sheet name="OR stunting by compfeeding" sheetId="17" r:id="rId17"/>
+    <sheet name="OR correctBF by interventn" sheetId="18" r:id="rId18"/>
     <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId19"/>
     <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId20"/>
     <sheet name="Interventions target population" sheetId="21" r:id="rId21"/>
@@ -429,9 +429,6 @@
     <t>Intervention</t>
   </si>
   <si>
-    <t>Complements group</t>
-  </si>
-  <si>
     <t>Complementary feeding (food secure with promotion)</t>
   </si>
   <si>
@@ -496,6 +493,9 @@
   </si>
   <si>
     <t>Balanced energy-protein supplementation</t>
+  </si>
+  <si>
+    <t>Food security &amp; education</t>
   </si>
 </sst>
 </file>
@@ -1222,6 +1222,108 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1592,7 +1694,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="13">
         <v>0.56799999999999995</v>
@@ -1600,7 +1702,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="26">
         <v>0.4</v>
@@ -1608,7 +1710,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="26">
         <v>0.20599999999999999</v>
@@ -2825,7 +2927,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
@@ -2886,7 +2988,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -2906,7 +3008,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="6">
         <v>1</v>
@@ -2926,7 +3028,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="6">
         <v>1</v>
@@ -2946,7 +3048,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -2966,7 +3068,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -3025,7 +3127,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="18">
         <v>5.16</v>
@@ -3286,18 +3388,18 @@
         <v>56</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="20">
         <v>0</v>
@@ -3314,7 +3416,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="6">
         <v>0.621</v>
@@ -3331,7 +3433,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="6">
         <v>0.247</v>
@@ -3348,7 +3450,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="6">
         <v>0</v>
@@ -3365,7 +3467,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="6">
         <v>0.61</v>
@@ -3382,7 +3484,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="6">
         <v>0</v>
@@ -3399,7 +3501,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -3554,14 +3656,14 @@
         <v>15</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -3584,7 +3686,7 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -3607,7 +3709,7 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3630,7 +3732,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -3655,7 +3757,7 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="4">
         <v>1</v>
@@ -3678,7 +3780,7 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -3702,7 +3804,7 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="4">
         <v>0</v>
@@ -3845,7 +3947,7 @@
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>23</v>
@@ -3862,10 +3964,10 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="23">
         <v>0.21</v>
@@ -3882,7 +3984,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="23">
         <f>demographics!$B$5 * 'Interventions target population'!$G$7</f>
@@ -3901,10 +4003,10 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="23">
         <v>0.1</v>
@@ -3921,7 +4023,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="23">
         <v>1</v>
@@ -3956,7 +4058,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>10</v>
@@ -3979,7 +4081,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
@@ -4023,7 +4125,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>34</v>
@@ -4105,7 +4207,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>10</v>
@@ -4128,7 +4230,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
@@ -4172,7 +4274,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>34</v>
@@ -4243,7 +4345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
@@ -4254,7 +4356,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>10</v>
@@ -4277,7 +4379,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>34</v>
@@ -4321,7 +4423,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>34</v>
@@ -5210,7 +5312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>

</xml_diff>